<commit_message>
refactor: Lean BI - Remove redundant charts and simplify PIM-PF filters
- Remove YoY and YTD charts from Atividade Industrial page
- Promote Activity Level Index chart to central position
- Rename ranking section to 'Competitividade Regional'
- Simplify macro filters to match IBGE PIM-PF API capabilities (State + Division only)
- Add educational note about PIM-PF data granularity limitations
- Security: No sensitive data exposed, .gitignore properly configured
</commit_message>
<xml_diff>
--- a/CNAE_Subclasses_2_3_Estrutura_Detalhada.xlsx
+++ b/CNAE_Subclasses_2_3_Estrutura_Detalhada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ercaavi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ercaavi\Downloads\Nexus-Industrial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C922AF-66B1-449F-ACB2-7007533E5FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5A1AEF-1A5D-4FF5-914C-987CD7A6C5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estrutura Det. CNAE Subclass2.3" sheetId="1" r:id="rId1"/>
@@ -13835,6 +13835,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -13856,13 +13866,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -13872,9 +13875,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -14293,8 +14293,8 @@
   </sheetPr>
   <dimension ref="A1:G2401"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M112" sqref="M112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -43151,9 +43151,6 @@
 CNAE-Subclasses 2.3</oddHeader>
     <oddFooter>&amp;C&amp;P&amp;R&amp;D</oddFooter>
   </headerFooter>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -43181,36 +43178,36 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="67" t="s">
         <v>4280</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65" t="s">
+      <c r="C2" s="68"/>
+      <c r="D2" s="68" t="s">
         <v>4281</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66" t="s">
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="69" t="s">
         <v>4283</v>
       </c>
     </row>
     <row r="3" spans="2:7" s="30" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="75" t="s">
         <v>4277</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="74" t="s">
         <v>4278</v>
       </c>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="67"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="64" t="s">
         <v>3764</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="76" t="s">
         <v>3765</v>
       </c>
       <c r="D4" s="31" t="s">
@@ -43223,8 +43220,8 @@
       <c r="G4" s="33"/>
     </row>
     <row r="5" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="72"/>
-      <c r="C5" s="71"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="34" t="s">
         <v>4224</v>
       </c>
@@ -43239,18 +43236,18 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="68"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="73"/>
     </row>
     <row r="7" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="65" t="s">
         <v>3766</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="66" t="s">
         <v>3767</v>
       </c>
       <c r="D7" s="34" t="s">
@@ -43263,8 +43260,8 @@
       <c r="G7" s="36"/>
     </row>
     <row r="8" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="72"/>
-      <c r="C8" s="71"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="34" t="s">
         <v>4224</v>
       </c>
@@ -43279,18 +43276,18 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="68"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="73"/>
     </row>
     <row r="10" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="65" t="s">
         <v>3665</v>
       </c>
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="66" t="s">
         <v>3666</v>
       </c>
       <c r="D10" s="34" t="s">
@@ -43303,8 +43300,8 @@
       <c r="G10" s="36"/>
     </row>
     <row r="11" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="72"/>
-      <c r="C11" s="71"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="34" t="s">
         <v>4239</v>
       </c>
@@ -43315,18 +43312,18 @@
       <c r="G11" s="36"/>
     </row>
     <row r="12" spans="2:7" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="68"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="70"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="73"/>
     </row>
     <row r="13" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="65" t="s">
         <v>2100</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="66" t="s">
         <v>2101</v>
       </c>
       <c r="D13" s="34" t="s">
@@ -43339,8 +43336,8 @@
       <c r="G13" s="36"/>
     </row>
     <row r="14" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="72"/>
-      <c r="C14" s="71"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="34" t="s">
         <v>4243</v>
       </c>
@@ -43355,12 +43352,12 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="68"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="70"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
     </row>
     <row r="16" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="37" t="s">
@@ -43383,18 +43380,18 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="68"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="73"/>
     </row>
     <row r="18" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="65" t="s">
         <v>4091</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="66" t="s">
         <v>4092</v>
       </c>
       <c r="D18" s="34" t="s">
@@ -43407,8 +43404,8 @@
       <c r="G18" s="36"/>
     </row>
     <row r="19" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="72"/>
-      <c r="C19" s="71"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
       <c r="D19" s="34" t="s">
         <v>4248</v>
       </c>
@@ -43419,12 +43416,12 @@
       <c r="G19" s="36"/>
     </row>
     <row r="20" spans="2:7" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="68"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="70"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="73"/>
     </row>
     <row r="21" spans="2:7" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="39" t="s">
@@ -43446,11 +43443,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B10:B11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:G3"/>
@@ -43467,6 +43459,11 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>